<commit_message>
menage + class + recalcul
</commit_message>
<xml_diff>
--- a/matrice_temps/demo.xlsx
+++ b/matrice_temps/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Equipes</t>
   </si>
@@ -34,54 +34,48 @@
     <t>K. Bryant</t>
   </si>
   <si>
+    <t>R. Federer</t>
+  </si>
+  <si>
+    <t>P. Mickelson</t>
+  </si>
+  <si>
+    <t>R. Nadal</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
-    <t>R. Federer</t>
-  </si>
-  <si>
-    <t>P. Mickelson</t>
-  </si>
-  <si>
-    <t>R. Nadal</t>
-  </si>
-  <si>
     <t>M. Ryan</t>
   </si>
   <si>
+    <t>M. Pacquiao</t>
+  </si>
+  <si>
+    <t>Z. Ibrahimović</t>
+  </si>
+  <si>
+    <t>D. Rose</t>
+  </si>
+  <si>
+    <t>G. Bale</t>
+  </si>
+  <si>
+    <t>R. Falcao</t>
+  </si>
+  <si>
+    <t>M. Özil</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>M. Pacquiao</t>
-  </si>
-  <si>
-    <t>Z. Ibrahimović</t>
-  </si>
-  <si>
-    <t>D. Rose</t>
-  </si>
-  <si>
-    <t>G. Bale</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>R. Falcao</t>
-  </si>
-  <si>
-    <t>M. Özil</t>
-  </si>
-  <si>
     <t>N. Djokovic</t>
   </si>
   <si>
     <t>M. Stafford</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>L. Hamilton</t>
   </si>
   <si>
@@ -92,6 +86,9 @@
   </si>
   <si>
     <t>M. Singh</t>
+  </si>
+  <si>
+    <t>D. Wade</t>
   </si>
 </sst>
 </file>
@@ -432,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +438,7 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,84 +446,87 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
repartition des menbres dans chaque equipe. 7/7/4 -> 6/6/6
</commit_message>
<xml_diff>
--- a/matrice_temps/demo.xlsx
+++ b/matrice_temps/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Equipes</t>
   </si>
@@ -40,12 +40,12 @@
     <t>P. Mickelson</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>R. Nadal</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>M. Ryan</t>
   </si>
   <si>
@@ -61,15 +61,15 @@
     <t>G. Bale</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>R. Falcao</t>
   </si>
   <si>
     <t>M. Özil</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>N. Djokovic</t>
   </si>
   <si>
@@ -80,15 +80,6 @@
   </si>
   <si>
     <t>K. Durant</t>
-  </si>
-  <si>
-    <t>F. Alonso</t>
-  </si>
-  <si>
-    <t>M. Singh</t>
-  </si>
-  <si>
-    <t>D. Wade</t>
   </si>
 </sst>
 </file>
@@ -429,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -446,10 +437,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -457,10 +448,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -468,10 +459,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -479,10 +470,10 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -490,10 +481,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -501,10 +492,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -512,21 +503,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>